<commit_message>
modified:   homeworkchecker v2.5.py 	modified:   "\346\265\213\350\257\225\346\225\260\346\215\256\346\272\220/answer.xlsx"
</commit_message>
<xml_diff>
--- a/测试数据源/answer.xlsx
+++ b/测试数据源/answer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\看作业系统\测试数据源\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D8CD4D-D31B-475A-9BE9-428049F494EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604A25E5-8EC6-4424-8FFE-10A8D1A3905B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2952" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3432" yWindow="1896" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,55 +381,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -437,5 +440,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>